<commit_message>
update file excel SM400
</commit_message>
<xml_diff>
--- a/docs/assets/images/integrated-devices/smc/sm400/statistics-of-storage-memory-device.xlsx
+++ b/docs/assets/images/integrated-devices/smc/sm400/statistics-of-storage-memory-device.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>STATISTICS OF DATA TRANSMISSION BY DEVICE S400</t>
   </si>
@@ -222,12 +222,6 @@
     <t>Total Consumption (MB)</t>
   </si>
   <si>
-    <t>THỐNG KÊ  BỘ NHỚ LƯU TRỮ DỮ LIỆU BỞI THIẾT BỊ SM400</t>
-  </si>
-  <si>
-    <t>Lưu ý: bảng này được lập ra dựa trên tính toán theo mẫu hoạt động mặc định mà nhà sản xuất cài đặt khi xuất xưởng.</t>
-  </si>
-  <si>
     <t>Storage (MB) / day</t>
   </si>
   <si>
@@ -379,6 +373,9 @@
   </si>
   <si>
     <t>Total Storage (GB)</t>
+  </si>
+  <si>
+    <t>STATISTICS OF DATA TRANSMISSION BY DEVICE SM400</t>
   </si>
 </sst>
 </file>
@@ -571,7 +568,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -652,12 +649,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -884,7 +875,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -7017,7 +7008,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -7032,8 +7023,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="23.25" customHeight="1">
-      <c r="A1" s="33" t="s">
-        <v>15</v>
+      <c r="A1" s="23" t="s">
+        <v>22</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -7052,8 +7043,8 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="23.25" customHeight="1">
-      <c r="A3" s="34" t="s">
-        <v>16</v>
+      <c r="A3" s="29" t="s">
+        <v>1</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
@@ -7076,7 +7067,7 @@
         <v>5</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>7</v>
@@ -7107,10 +7098,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="13">
         <v>1</v>
@@ -7130,10 +7121,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" s="13">
         <v>1</v>
@@ -7149,8 +7140,8 @@
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:26" ht="33" customHeight="1">
-      <c r="A7" s="35" t="s">
-        <v>22</v>
+      <c r="A7" s="33" t="s">
+        <v>20</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="30"/>
@@ -7163,8 +7154,8 @@
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="33" customHeight="1">
-      <c r="A8" s="35" t="s">
-        <v>23</v>
+      <c r="A8" s="33" t="s">
+        <v>21</v>
       </c>
       <c r="B8" s="30"/>
       <c r="C8" s="30"/>

</xml_diff>